<commit_message>
permitir professor bloquear a profa; alterei a forma de apresentacao das datas da avaliacao ao criar/editar; corrigi o bug de selecionar alunos; melhorei mecanismo de pesquisa no selecionar alunos
</commit_message>
<xml_diff>
--- a/TAREFAS.xlsx
+++ b/TAREFAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfabini\Google Drive\MySoftwares\Angular\ProjetoTCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AF9B00-33A5-4E66-89BF-A0BBDCE16A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E418AA-594F-46F1-A8B9-3AEC57144D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83B462A5-D076-40C0-9EB2-135E6AFA7A23}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Confirmar Dialog: Colocar no título o que está ocorrendo ao invés de "Atenção"</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>DURAÇÃO REAL</t>
+  </si>
+  <si>
+    <t>feito</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -161,11 +164,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -192,12 +208,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,8 +538,8 @@
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,13 +563,13 @@
       <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -557,11 +579,11 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B3" s="11">
+      <c r="B3" s="13">
         <v>44123</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="2:7" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
@@ -675,11 +697,11 @@
       <c r="E9" s="9"/>
     </row>
     <row r="10" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B10" s="11">
+      <c r="B10" s="13">
         <v>44124</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -692,6 +714,13 @@
       <c r="D11" s="3">
         <v>2</v>
       </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
@@ -703,7 +732,16 @@
       <c r="D12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="2">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" ref="G12" si="1">F12-E12</f>
+        <v>0.17013888888888895</v>
+      </c>
     </row>
     <row r="13" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
@@ -715,8 +753,13 @@
       <c r="D13" s="3">
         <v>2</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="G13" s="10" t="s">
+      <c r="E13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -730,7 +773,9 @@
       <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7" ht="26" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
@@ -739,13 +784,13 @@
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B16" s="11">
+      <c r="B16" s="13">
         <v>44125</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="2:5" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="2:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
@@ -755,8 +800,11 @@
       <c r="D17" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="2:7" ht="26" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
@@ -766,9 +814,11 @@
       <c r="D18" s="3">
         <v>3</v>
       </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E18" s="12"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
@@ -778,9 +828,11 @@
       <c r="D19" s="3">
         <v>3</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E19" s="12"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="2:7" ht="26" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
@@ -790,9 +842,11 @@
       <c r="D20" s="3">
         <v>3</v>
       </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="E20" s="12"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
@@ -802,8 +856,11 @@
       <c r="D21" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
@@ -813,6 +870,9 @@
       <c r="D22" s="3">
         <v>2</v>
       </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Adicionei funções para anexos
</commit_message>
<xml_diff>
--- a/TAREFAS.xlsx
+++ b/TAREFAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfabini\Google Drive\MySoftwares\Angular\ProjetoTCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E418AA-594F-46F1-A8B9-3AEC57144D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBA646B-370D-405C-AA11-D4EB47AE43BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83B462A5-D076-40C0-9EB2-135E6AFA7A23}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Confirmar Dialog: Colocar no título o que está ocorrendo ao invés de "Atenção"</t>
   </si>
@@ -538,8 +538,8 @@
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,8 +773,12 @@
       <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7" ht="26" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Adicionei cronometro; ajuda ao criar avaliacoes; validações; melhoria na dinamica de criar questao;
</commit_message>
<xml_diff>
--- a/TAREFAS.xlsx
+++ b/TAREFAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfabini\Google Drive\MySoftwares\Angular\ProjetoTCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBA646B-370D-405C-AA11-D4EB47AE43BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3136E214-6C92-46CB-AACC-B39B6FA4AD5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83B462A5-D076-40C0-9EB2-135E6AFA7A23}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Confirmar Dialog: Colocar no título o que está ocorrendo ao invés de "Atenção"</t>
   </si>
@@ -212,13 +212,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -538,8 +538,8 @@
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,11 +579,11 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>44123</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="2:7" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
@@ -697,11 +697,11 @@
       <c r="E9" s="9"/>
     </row>
     <row r="10" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>44124</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -788,11 +788,11 @@
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <v>44125</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
@@ -804,11 +804,15 @@
       <c r="D17" s="3">
         <v>1</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="2:7" ht="26" x14ac:dyDescent="0.35">
+      <c r="E17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="2:7" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
@@ -818,9 +822,13 @@
       <c r="D18" s="3">
         <v>3</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
@@ -832,9 +840,13 @@
       <c r="D19" s="3">
         <v>3</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="E19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" ht="26" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
@@ -846,9 +858,13 @@
       <c r="D20" s="3">
         <v>3</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="E20" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
@@ -860,9 +876,9 @@
       <c r="D21" s="3">
         <v>2</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
@@ -874,9 +890,9 @@
       <c r="D22" s="3">
         <v>2</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Adicionei função para que Quando o componente avaliacao-professor estiver com avalicao status 2 ou 3, já deve passar por cada prova e atribuindo a nota padrão; Corrigir bug de simultaniedade ao: alterar status do alunos; alterar status da avaliação; alterar nota/correção das provas;
</commit_message>
<xml_diff>
--- a/TAREFAS.xlsx
+++ b/TAREFAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfabini\Google Drive\MySoftwares\Angular\ProjetoTCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3136E214-6C92-46CB-AACC-B39B6FA4AD5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A99EE3C-A145-4D93-8342-4D79CC588611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83B462A5-D076-40C0-9EB2-135E6AFA7A23}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$D$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$D$15</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -127,21 +127,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -164,24 +158,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -205,19 +186,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -535,21 +507,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68849C5F-715D-4E86-9C61-635F4EA8F9A5}">
-  <dimension ref="B1:G22"/>
+  <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="6"/>
     <col min="2" max="2" width="36.6328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" style="5" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="5" customWidth="1"/>
-    <col min="5" max="6" width="26.1796875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" style="6" customWidth="1"/>
+    <col min="5" max="6" width="26.1796875" style="6" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="6" hidden="1" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
@@ -563,13 +535,13 @@
       <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -578,180 +550,215 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B3" s="12">
-        <v>44123</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="2:7" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.25486111111111109</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.25763888888888892</v>
+      </c>
+      <c r="G3" s="2">
+        <f>F3-E3</f>
+        <v>2.7777777777778234E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>1.0416666666666666E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>0.25486111111111109</v>
+        <v>0.25833333333333336</v>
       </c>
       <c r="F4" s="2">
-        <v>0.25763888888888892</v>
+        <v>0.26250000000000001</v>
       </c>
       <c r="G4" s="2">
-        <f>F4-E4</f>
-        <v>2.7777777777778234E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+        <f t="shared" ref="G4:G7" si="0">F4-E4</f>
+        <v>4.1666666666666519E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>6.9444444444444441E-3</v>
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>0.25833333333333336</v>
+        <v>0.26319444444444445</v>
       </c>
       <c r="F5" s="2">
-        <v>0.26250000000000001</v>
+        <v>0.27708333333333335</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G8" si="0">F5-E5</f>
-        <v>4.1666666666666519E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>2.4305555555555556E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>0.26319444444444445</v>
+        <v>0.27916666666666667</v>
       </c>
       <c r="F6" s="2">
-        <v>0.27708333333333335</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>1.3888888888888895E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+        <f>F6-E6</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>4.1666666666666664E-2</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>0.27916666666666667</v>
+        <v>0.3840277777777778</v>
       </c>
       <c r="F7" s="2">
-        <v>0.35416666666666669</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="G7" s="2">
-        <f>F7-E7</f>
-        <v>7.5000000000000011E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.15277777777777776</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.3840277777777778</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.49305555555555558</v>
-      </c>
-      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>0.10902777777777778</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B10" s="12">
-        <v>44124</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" ref="G9" si="1">F9-E9</f>
+        <v>0.17013888888888895</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="2:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="2:7" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D11" s="3">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D12" s="3">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.30208333333333331</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" ref="G12" si="1">F12-E12</f>
-        <v>0.17013888888888895</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
       <c r="D13" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>22</v>
@@ -759,148 +766,74 @@
       <c r="F13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
-        <v>0.1111111111111111</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B16" s="12">
-        <v>44125</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="2:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="D19" s="3">
-        <v>3</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="2:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D20" s="3">
-        <v>3</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="2:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="B21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D22" s="3">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <conditionalFormatting sqref="C17:C22 C11:C14 C4:C8">
+  <conditionalFormatting sqref="C3:C17">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>